<commit_message>
Add home button to payment
</commit_message>
<xml_diff>
--- a/frontend/public/student_bulk_upload_template.xlsx
+++ b/frontend/public/student_bulk_upload_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedamirshah/Desktop/Learnify Pakistan/upload excell docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedamirshah/Documents/learnify-clean/frontend/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D80D67E-20DC-934A-90BF-3DB8F48D59D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A7CCB1-4719-A54D-984B-D9F195E093DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="26360" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>username</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -656,6 +656,9 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
         <v>24</v>
       </c>

</xml_diff>